<commit_message>
Updates for figures 2 and 5 following editorial requests
</commit_message>
<xml_diff>
--- a/images/raw/sources.xlsx
+++ b/images/raw/sources.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7153ED-CC0E-4D9B-B95D-C823B82CCA3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="795" yWindow="435" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="top10hedge" sheetId="1" r:id="rId1"/>
@@ -147,12 +148,6 @@
     <t>Nandinia binotata</t>
   </si>
   <si>
-    <t>David Renoult</t>
-  </si>
-  <si>
-    <t>https://www.inaturalist.org/photos/10045047</t>
-  </si>
-  <si>
     <t>Vicente Valdes Guzman</t>
   </si>
   <si>
@@ -232,12 +227,18 @@
   </si>
   <si>
     <t>https://www.inaturalist.org/photos/53459059</t>
+  </si>
+  <si>
+    <t>https://www.inaturalist.org/photos/78448701</t>
+  </si>
+  <si>
+    <t>Dave Brown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -329,6 +330,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -376,7 +380,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -409,9 +413,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -444,6 +465,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -619,7 +657,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -762,11 +800,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,11 +830,11 @@
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>44</v>
+      <c r="B2" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -804,10 +842,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -815,10 +853,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -826,10 +864,10 @@
         <v>36</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -837,10 +875,10 @@
         <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -848,10 +886,10 @@
         <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -859,10 +897,10 @@
         <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -870,10 +908,10 @@
         <v>40</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -881,10 +919,10 @@
         <v>41</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -892,26 +930,27 @@
         <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{D142937E-1A27-4E47-A52E-D5FCD5417AEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -935,40 +974,40 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
         <v>69</v>
       </c>
-      <c r="B4" t="s">
-        <v>71</v>
-      </c>
       <c r="C4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>

</xml_diff>